<commit_message>
update bug rep. and test plan
</commit_message>
<xml_diff>
--- a/Testing/Bug Report.xlsx
+++ b/Testing/Bug Report.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internet-banking-system\Testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Logout" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="View Account" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Perform Transaction" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Close Account" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Add new Account" sheetId="7" r:id="rId10"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Logout" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="View Account" sheetId="4" r:id="rId4"/>
+    <sheet name="Perform Transaction" sheetId="5" r:id="rId5"/>
+    <sheet name="Close Account" sheetId="6" r:id="rId6"/>
+    <sheet name="Add new Account" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -63,23 +71,53 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <r>
+      <t>Environment details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -87,7 +125,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -97,56 +135,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -336,20 +362,96 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,21 +499,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,21 +562,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,21 +625,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,21 +688,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,21 +751,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,68 +814,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>